<commit_message>
Update Work Breackdown Structure.xlsx
i just modified some days, i put less days in crud and more in web based functions
</commit_message>
<xml_diff>
--- a/documents/Work Breackdown Structure.xlsx
+++ b/documents/Work Breackdown Structure.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">    CRUD</t>
   </si>
   <si>
-    <t xml:space="preserve">     13 Days</t>
+    <t xml:space="preserve">     8 Days</t>
   </si>
   <si>
     <t xml:space="preserve">   1.1.2.1</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">      Create communication to DB</t>
   </si>
   <si>
-    <t xml:space="preserve">       8 Days</t>
+    <t xml:space="preserve">       3 Days</t>
   </si>
   <si>
     <t xml:space="preserve">   1.1.2.2</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">    Create expecific Web functions</t>
   </si>
   <si>
-    <t xml:space="preserve">     9 Days</t>
+    <t xml:space="preserve">     14 Days</t>
   </si>
   <si>
     <t xml:space="preserve">  1.1.4</t>
@@ -1369,7 +1369,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="3"/>

</xml_diff>